<commit_message>
modify break peak condition
</commit_message>
<xml_diff>
--- a/src/main/resources/SH600318.xlsx
+++ b/src/main/resources/SH600318.xlsx
@@ -174,1771 +174,1771 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20020606</t>
+          <t>20020403</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>274.0</v>
+        <v>310.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20020625</t>
+          <t>20020411</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>345.0</v>
+        <v>343.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20020820</t>
+          <t>20020606</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>299.0</v>
+        <v>274.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20020902</t>
+          <t>20020625</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>312.0</v>
+        <v>345.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20020918</t>
+          <t>20020820</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>295.0</v>
+        <v>299.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20020920</t>
+          <t>20020902</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>314.0</v>
+        <v>312.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20021127</t>
+          <t>20020918</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>216.0</v>
+        <v>295.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20021204</t>
+          <t>20020920</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>248.0</v>
+        <v>314.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20021231</t>
+          <t>20021127</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>208.0</v>
+        <v>216.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20030304</t>
+          <t>20021204</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>263.0</v>
+        <v>248.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20030327</t>
+          <t>20021231</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>223.0</v>
+        <v>208.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20030402</t>
+          <t>20030304</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>238.0</v>
+        <v>263.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20030409</t>
+          <t>20030327</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>217.0</v>
+        <v>223.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20030418</t>
+          <t>20030402</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>248.0</v>
+        <v>238.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20030513</t>
+          <t>20030409</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>173.0</v>
+        <v>217.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20030526</t>
+          <t>20030418</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>217.0</v>
+        <v>248.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20030609</t>
+          <t>20030513</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>191.0</v>
+        <v>173.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20030702</t>
+          <t>20030526</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>213.0</v>
+        <v>217.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20030725</t>
+          <t>20030609</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>175.0</v>
+        <v>191.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20030811</t>
+          <t>20030702</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>196.0</v>
+        <v>213.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20030929</t>
+          <t>20030725</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>155.0</v>
+        <v>175.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20031024</t>
+          <t>20030811</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>180.0</v>
+        <v>196.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20031113</t>
+          <t>20030929</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>156.0</v>
+        <v>155.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20031203</t>
+          <t>20031024</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>183.0</v>
+        <v>180.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20031222</t>
+          <t>20031113</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>145.0</v>
+        <v>156.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20040302</t>
+          <t>20031203</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>284.0</v>
+        <v>183.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20040422</t>
+          <t>20031222</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>196.0</v>
+        <v>145.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20040519</t>
+          <t>20040302</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>269.0</v>
+        <v>284.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20040727</t>
+          <t>20040422</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>168.0</v>
+        <v>196.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20040729</t>
+          <t>20040519</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>183.0</v>
+        <v>269.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20040819</t>
+          <t>20040727</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>155.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20040831</t>
+          <t>20040729</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>170.0</v>
+        <v>183.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20040913</t>
+          <t>20040819</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>150.0</v>
+        <v>155.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20041014</t>
+          <t>20040831</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>209.0</v>
+        <v>170.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20041102</t>
+          <t>20040913</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>153.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20041124</t>
+          <t>20041014</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>177.0</v>
+        <v>209.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20041220</t>
+          <t>20041102</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>152.0</v>
+        <v>153.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20041231</t>
+          <t>20041124</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>168.0</v>
+        <v>177.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20050121</t>
+          <t>20041220</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>131.0</v>
+        <v>152.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20050315</t>
+          <t>20041231</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>203.0</v>
+        <v>168.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20050523</t>
+          <t>20050121</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>67.0</v>
+        <v>131.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20050613</t>
+          <t>20050315</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>95.0</v>
+        <v>203.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20050718</t>
+          <t>20050523</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>46.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20050919</t>
+          <t>20050613</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>120.0</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20051010</t>
+          <t>20050718</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>76.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20051021</t>
+          <t>20050919</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>98.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20051101</t>
+          <t>20051010</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>69.0</v>
+        <v>76.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20060116</t>
+          <t>20051021</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>101.0</v>
+        <v>98.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20060125</t>
+          <t>20051101</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>77.0</v>
+        <v>69.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>20060404</t>
+          <t>20060116</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>127.0</v>
+        <v>101.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20060425</t>
+          <t>20060125</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>104.0</v>
+        <v>77.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20060518</t>
+          <t>20060404</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>274.0</v>
+        <v>127.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20060619</t>
+          <t>20060425</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>162.0</v>
+        <v>104.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20060711</t>
+          <t>20060518</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>218.0</v>
+        <v>274.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20060807</t>
+          <t>20060619</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>128.0</v>
+        <v>162.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20060921</t>
+          <t>20060711</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>181.0</v>
+        <v>218.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>20061030</t>
+          <t>20060807</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>134.0</v>
+        <v>128.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>20070420</t>
+          <t>20060921</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>556.0</v>
+        <v>181.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>20070719</t>
+          <t>20061030</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>343.0</v>
+        <v>134.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20070731</t>
+          <t>20070420</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>628.0</v>
+        <v>556.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20070813</t>
+          <t>20070719</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>448.0</v>
+        <v>343.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20070822</t>
+          <t>20070731</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>528.0</v>
+        <v>628.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>20070912</t>
+          <t>20070813</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>438.0</v>
+        <v>448.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>20071008</t>
+          <t>20070822</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>573.0</v>
+        <v>528.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>20071029</t>
+          <t>20070912</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>327.0</v>
+        <v>438.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>20080117</t>
+          <t>20071008</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>787.0</v>
+        <v>573.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>20080201</t>
+          <t>20071029</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>478.0</v>
+        <v>327.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>20080219</t>
+          <t>20080117</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>706.0</v>
+        <v>787.0</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>20080422</t>
+          <t>20080201</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>339.0</v>
+        <v>478.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>20080520</t>
+          <t>20080219</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>553.0</v>
+        <v>706.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>20080620</t>
+          <t>20080422</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>229.0</v>
+        <v>339.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>20080710</t>
+          <t>20080520</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>330.0</v>
+        <v>553.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>20080718</t>
+          <t>20080620</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>255.0</v>
+        <v>229.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>20080725</t>
+          <t>20080710</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>322.0</v>
+        <v>330.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>20080819</t>
+          <t>20080718</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>173.0</v>
+        <v>255.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>20080901</t>
+          <t>20080725</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>225.0</v>
+        <v>322.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>20080918</t>
+          <t>20080819</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>152.0</v>
+        <v>173.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>20080922</t>
+          <t>20080901</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>197.0</v>
+        <v>225.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>20081104</t>
+          <t>20080918</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>109.0</v>
+        <v>152.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>20081209</t>
+          <t>20080922</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>238.0</v>
+        <v>197.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>20081224</t>
+          <t>20081104</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>178.0</v>
+        <v>109.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>20090224</t>
+          <t>20081209</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>326.0</v>
+        <v>238.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>20090302</t>
+          <t>20081224</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>229.0</v>
+        <v>178.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>20090422</t>
+          <t>20090224</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>426.0</v>
+        <v>326.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>20090428</t>
+          <t>20090302</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>340.0</v>
+        <v>229.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>20090506</t>
+          <t>20090422</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>412.0</v>
+        <v>426.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>20090525</t>
+          <t>20090428</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>335.0</v>
+        <v>340.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>20090605</t>
+          <t>20090506</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>387.0</v>
+        <v>412.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>20090701</t>
+          <t>20090525</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>334.0</v>
+        <v>335.0</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>20090724</t>
+          <t>20090605</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>489.0</v>
+        <v>387.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>20090819</t>
+          <t>20090701</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>341.0</v>
+        <v>334.0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>20091124</t>
+          <t>20090724</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>459.0</v>
+        <v>489.0</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>20091222</t>
+          <t>20090819</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>365.0</v>
+        <v>341.0</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>20100119</t>
+          <t>20091124</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>446.0</v>
+        <v>459.0</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>20100127</t>
+          <t>20091222</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>370.0</v>
+        <v>365.0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>20100301</t>
+          <t>20100119</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>469.0</v>
+        <v>446.0</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>20100315</t>
+          <t>20100127</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>405.0</v>
+        <v>370.0</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>20100416</t>
+          <t>20100301</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>489.0</v>
+        <v>469.0</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>20100519</t>
+          <t>20100315</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>313.0</v>
+        <v>405.0</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>20100608</t>
+          <t>20100416</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>378.0</v>
+        <v>489.0</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>20100702</t>
+          <t>20100519</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>266.0</v>
+        <v>313.0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>20100909</t>
+          <t>20100608</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>457.0</v>
+        <v>378.0</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>20100920</t>
+          <t>20100702</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>374.0</v>
+        <v>266.0</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>20101215</t>
+          <t>20100909</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>660.0</v>
+        <v>457.0</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>20101229</t>
+          <t>20100920</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>528.0</v>
+        <v>374.0</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>20110107</t>
+          <t>20101215</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>697.0</v>
+        <v>660.0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>20110118</t>
+          <t>20101229</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>594.0</v>
+        <v>528.0</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>20110304</t>
+          <t>20110107</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>927.0</v>
+        <v>697.0</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>20110315</t>
+          <t>20110118</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>784.0</v>
+        <v>594.0</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>20110407</t>
+          <t>20110304</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>1111.0</v>
+        <v>927.0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>20110426</t>
+          <t>20110315</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>905.0</v>
+        <v>784.0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>20110504</t>
+          <t>20110407</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>1047.0</v>
+        <v>1111.0</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>20110531</t>
+          <t>20110426</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>754.0</v>
+        <v>905.0</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>20110715</t>
+          <t>20110504</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>1162.0</v>
+        <v>1047.0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>20111219</t>
+          <t>20110531</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>475.0</v>
+        <v>754.0</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>20120118</t>
+          <t>20110715</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>668.0</v>
+        <v>1162.0</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>20120201</t>
+          <t>20111219</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>578.0</v>
+        <v>475.0</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>20120224</t>
+          <t>20120118</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>727.0</v>
+        <v>668.0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>20120330</t>
+          <t>20120201</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>534.0</v>
+        <v>578.0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>20120425</t>
+          <t>20120224</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>667.0</v>
+        <v>727.0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>20120518</t>
+          <t>20120330</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>553.0</v>
+        <v>534.0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>20120529</t>
+          <t>20120425</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>707.0</v>
+        <v>667.0</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>20120731</t>
+          <t>20120518</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>433.0</v>
+        <v>553.0</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>20120808</t>
+          <t>20120529</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>493.0</v>
+        <v>707.0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>20120828</t>
+          <t>20120731</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>437.0</v>
+        <v>433.0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>20120910</t>
+          <t>20120808</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>578.0</v>
+        <v>493.0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>20120924</t>
+          <t>20120828</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>443.0</v>
+        <v>437.0</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>20121019</t>
+          <t>20120910</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>542.0</v>
+        <v>578.0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>20121129</t>
+          <t>20120924</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>384.0</v>
+        <v>443.0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>20130218</t>
+          <t>20121019</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>684.0</v>
+        <v>542.0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>20130318</t>
+          <t>20121129</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>464.0</v>
+        <v>384.0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>20130422</t>
+          <t>20130218</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>608.0</v>
+        <v>684.0</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>20130516</t>
+          <t>20130318</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>485.0</v>
+        <v>464.0</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>20130613</t>
+          <t>20130422</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>657.0</v>
+        <v>608.0</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>20130701</t>
+          <t>20130516</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>509.0</v>
+        <v>485.0</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>20130711</t>
+          <t>20130613</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>610.0</v>
+        <v>657.0</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>20130730</t>
+          <t>20130701</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>435.0</v>
+        <v>509.0</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>20130813</t>
+          <t>20130711</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>535.0</v>
+        <v>610.0</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>20130819</t>
+          <t>20130730</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>469.0</v>
+        <v>435.0</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>20130911</t>
+          <t>20130813</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>532.0</v>
+        <v>535.0</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>20131029</t>
+          <t>20130819</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>401.0</v>
+        <v>469.0</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>20131204</t>
+          <t>20130911</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>543.0</v>
+        <v>532.0</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>20140120</t>
+          <t>20131029</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>394.0</v>
+        <v>401.0</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>20140219</t>
+          <t>20131204</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>451.0</v>
+        <v>543.0</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>20140228</t>
+          <t>20140120</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>389.0</v>
+        <v>394.0</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>20140410</t>
+          <t>20140219</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>450.0</v>
+        <v>451.0</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>20140425</t>
+          <t>20140228</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>400.0</v>
+        <v>389.0</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>20140610</t>
+          <t>20140410</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>451.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>20140619</t>
+          <t>20140425</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>401.0</v>
+        <v>400.0</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>20140915</t>
+          <t>20140610</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>546.0</v>
+        <v>451.0</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>20140922</t>
+          <t>20140619</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>515.0</v>
+        <v>401.0</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>20150310</t>
+          <t>20140915</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>1963.0</v>
+        <v>546.0</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>20150421</t>
+          <t>20140922</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>1343.0</v>
+        <v>515.0</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>20150528</t>
+          <t>20150310</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>2181.0</v>
+        <v>1963.0</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>20150709</t>
+          <t>20150421</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>631.0</v>
+        <v>1343.0</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>20151126</t>
+          <t>20150528</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>1968.0</v>
+        <v>2181.0</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>20160127</t>
+          <t>20150709</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>964.0</v>
+        <v>631.0</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>20160218</t>
+          <t>20151126</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>1417.0</v>
+        <v>1968.0</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>20160229</t>
+          <t>20160127</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>1033.0</v>
+        <v>964.0</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>20160923</t>
+          <t>20160218</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>1852.0</v>
+        <v>1417.0</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>20160930</t>
+          <t>20160229</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>1464.0</v>
+        <v>1033.0</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>20161107</t>
+          <t>20160923</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>1800.0</v>
+        <v>1852.0</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>20170116</t>
+          <t>20160930</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>1297.0</v>
+        <v>1464.0</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>20170206</t>
+          <t>20161107</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>1533.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>20170217</t>
+          <t>20170116</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>1419.0</v>
+        <v>1297.0</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>20170222</t>
+          <t>20170206</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>1606.0</v>
+        <v>1533.0</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>20170424</t>
+          <t>20170217</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>1043.0</v>
+        <v>1419.0</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>20170919</t>
+          <t>20170222</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>1496.0</v>
+        <v>1606.0</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>20171020</t>
+          <t>20170424</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>1264.0</v>
+        <v>1043.0</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>20171108</t>
+          <t>20170919</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>1415.0</v>
+        <v>1496.0</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>20171127</t>
+          <t>20171020</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>1049.0</v>
+        <v>1264.0</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>20171227</t>
+          <t>20171108</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>1413.0</v>
+        <v>1415.0</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20171127</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>1054.0</v>
+        <v>1049.0</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>20180302</t>
+          <t>20171227</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>1246.0</v>
+        <v>1413.0</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>20181019</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B186" t="n">
-        <v>544.0</v>
+        <v>1054.0</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>20181031</t>
+          <t>20180302</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>848.0</v>
+        <v>1246.0</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>20181121</t>
+          <t>20181019</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>693.0</v>
+        <v>544.0</v>
       </c>
     </row>
     <row r="189">

</xml_diff>